<commit_message>
update melhora filtro lista drop
</commit_message>
<xml_diff>
--- a/quantidades_sem_cadeiras.xlsx
+++ b/quantidades_sem_cadeiras.xlsx
@@ -703,16 +703,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>43833</v>
+        <v>43663</v>
       </c>
       <c r="C16">
         <v>34089</v>
       </c>
       <c r="D16">
-        <v>9744</v>
+        <v>9574</v>
       </c>
       <c r="E16">
-        <v>77.77017315721032</v>
+        <v>78.07296795914161</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>